<commit_message>
added abs experiment data
</commit_message>
<xml_diff>
--- a/data_raw/input.xlsx
+++ b/data_raw/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11214"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nobuakiohsumi/Lec_handson/wtrwks_rpt/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDCAEA4-727B-DE42-8415-652075A21B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E73E04A-86C8-FC47-B7E0-5D3113089072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="5" xr2:uid="{11D640DA-DCFB-E544-8ADF-BF4092E26F00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="7" xr2:uid="{11D640DA-DCFB-E544-8ADF-BF4092E26F00}"/>
   </bookViews>
   <sheets>
     <sheet name="colony" sheetId="3" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="ozone_calib" sheetId="1" r:id="rId4"/>
     <sheet name="ozone" sheetId="2" r:id="rId5"/>
     <sheet name="manometer" sheetId="6" r:id="rId6"/>
+    <sheet name="abs_calib" sheetId="7" r:id="rId7"/>
+    <sheet name="abs" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="97">
   <si>
     <t>班</t>
   </si>
@@ -271,6 +273,114 @@
     <t>tapwtr</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>MB_conc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>day</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>group</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>crbn_amt</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>crbn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GW</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_0min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_0min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_5min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_20min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_30min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_60min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_90min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_120min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_24hrs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dil_10min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_5min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_10min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_20min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_30min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_60min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_90min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_120min</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ABS_24hrs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GLW</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MB_init_conc</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
@@ -310,7 +420,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,6 +431,18 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8E8E8"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -338,7 +460,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -358,6 +480,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5609,7 +5740,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -7538,7 +7669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70F5089C-337D-AB4E-A123-8CEBB17E04D3}">
   <dimension ref="A1:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="113" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -9518,4 +9649,1693 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B8D198-DF4E-5A4D-80C0-879C2B2FE6E1}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView zoomScale="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0.2</v>
+      </c>
+      <c r="D3">
+        <v>3.5999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0.5</v>
+      </c>
+      <c r="D4">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>0.435</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1.0509999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>1.958</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>3.2559999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>0.2</v>
+      </c>
+      <c r="D10">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>0.112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>0.44600000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>1.0429999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>1.958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>3.35</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F043729-32A1-B842-8BA1-3C91CFC99C7F}">
+  <dimension ref="A1:V33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" t="s">
+        <v>90</v>
+      </c>
+      <c r="J1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K1" t="s">
+        <v>92</v>
+      </c>
+      <c r="L1" t="s">
+        <v>93</v>
+      </c>
+      <c r="M1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N1" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" t="s">
+        <v>79</v>
+      </c>
+      <c r="P1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R1" t="s">
+        <v>81</v>
+      </c>
+      <c r="S1" t="s">
+        <v>82</v>
+      </c>
+      <c r="T1" t="s">
+        <v>83</v>
+      </c>
+      <c r="U1" t="s">
+        <v>84</v>
+      </c>
+      <c r="V1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2">
+        <v>400</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="8">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="M2">
+        <v>0.94599999999999995</v>
+      </c>
+      <c r="N2">
+        <v>100</v>
+      </c>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="8">
+        <v>100</v>
+      </c>
+      <c r="V2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <v>400</v>
+      </c>
+      <c r="D3">
+        <v>0.50029999999999997</v>
+      </c>
+      <c r="E3">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="F3">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="G3">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="H3">
+        <v>0.85099999999999998</v>
+      </c>
+      <c r="I3">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="J3">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="K3">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="L3">
+        <v>0.77200000000000002</v>
+      </c>
+      <c r="M3">
+        <v>0.60499999999999998</v>
+      </c>
+      <c r="N3">
+        <v>100</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
+      <c r="P3">
+        <v>100</v>
+      </c>
+      <c r="Q3">
+        <v>100</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+      <c r="S3">
+        <v>100</v>
+      </c>
+      <c r="T3">
+        <v>100</v>
+      </c>
+      <c r="U3">
+        <v>100</v>
+      </c>
+      <c r="V3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4">
+        <v>400</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="F4">
+        <v>0.8</v>
+      </c>
+      <c r="G4">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="H4">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="I4">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="J4">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="K4">
+        <v>0.623</v>
+      </c>
+      <c r="L4">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="M4">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="N4">
+        <v>100</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>100</v>
+      </c>
+      <c r="Q4">
+        <v>100</v>
+      </c>
+      <c r="R4">
+        <v>100</v>
+      </c>
+      <c r="S4">
+        <v>100</v>
+      </c>
+      <c r="T4">
+        <v>100</v>
+      </c>
+      <c r="U4">
+        <v>100</v>
+      </c>
+      <c r="V4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5">
+        <v>400</v>
+      </c>
+      <c r="D5">
+        <v>1.5015000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="G5">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="H5">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="I5">
+        <v>0.71399999999999997</v>
+      </c>
+      <c r="J5">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="K5">
+        <v>0.58799999999999997</v>
+      </c>
+      <c r="L5">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="M5">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="N5">
+        <v>100</v>
+      </c>
+      <c r="O5">
+        <v>100</v>
+      </c>
+      <c r="P5">
+        <v>100</v>
+      </c>
+      <c r="Q5">
+        <v>100</v>
+      </c>
+      <c r="R5">
+        <v>100</v>
+      </c>
+      <c r="S5">
+        <v>100</v>
+      </c>
+      <c r="T5">
+        <v>100</v>
+      </c>
+      <c r="U5">
+        <v>100</v>
+      </c>
+      <c r="V5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6">
+        <v>400</v>
+      </c>
+      <c r="D6">
+        <v>2.0070000000000001</v>
+      </c>
+      <c r="E6">
+        <v>0.878</v>
+      </c>
+      <c r="F6">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.73599999999999999</v>
+      </c>
+      <c r="H6">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="I6">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="J6">
+        <v>0.56899999999999995</v>
+      </c>
+      <c r="K6">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="L6">
+        <v>0.45800000000000002</v>
+      </c>
+      <c r="M6">
+        <v>1.5169999999999999</v>
+      </c>
+      <c r="N6">
+        <v>100</v>
+      </c>
+      <c r="O6">
+        <v>100</v>
+      </c>
+      <c r="P6">
+        <v>100</v>
+      </c>
+      <c r="Q6">
+        <v>100</v>
+      </c>
+      <c r="R6">
+        <v>100</v>
+      </c>
+      <c r="S6">
+        <v>100</v>
+      </c>
+      <c r="T6">
+        <v>100</v>
+      </c>
+      <c r="U6">
+        <v>100</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7">
+        <v>0.47799999999999998</v>
+      </c>
+      <c r="M7">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="N7">
+        <v>100</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7">
+        <v>100</v>
+      </c>
+      <c r="V7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>0.25</v>
+      </c>
+      <c r="E8">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="G8">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="H8">
+        <v>0.442</v>
+      </c>
+      <c r="I8">
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="J8">
+        <v>0.42799999999999999</v>
+      </c>
+      <c r="K8">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="L8">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="M8">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="N8">
+        <v>100</v>
+      </c>
+      <c r="O8">
+        <v>100</v>
+      </c>
+      <c r="P8">
+        <v>100</v>
+      </c>
+      <c r="Q8">
+        <v>100</v>
+      </c>
+      <c r="R8">
+        <v>100</v>
+      </c>
+      <c r="S8">
+        <v>100</v>
+      </c>
+      <c r="T8">
+        <v>100</v>
+      </c>
+      <c r="U8">
+        <v>100</v>
+      </c>
+      <c r="V8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>0.49980000000000002</v>
+      </c>
+      <c r="E9">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F9">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="G9">
+        <v>0.44600000000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.42</v>
+      </c>
+      <c r="I9">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="J9">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="K9">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.374</v>
+      </c>
+      <c r="M9">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="N9">
+        <v>100</v>
+      </c>
+      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="Q9">
+        <v>100</v>
+      </c>
+      <c r="R9">
+        <v>100</v>
+      </c>
+      <c r="S9">
+        <v>100</v>
+      </c>
+      <c r="T9">
+        <v>100</v>
+      </c>
+      <c r="U9">
+        <v>100</v>
+      </c>
+      <c r="V9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="F10">
+        <v>0.42399999999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="H10">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="J10">
+        <v>0.31900000000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="L10">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="M10">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="N10">
+        <v>100</v>
+      </c>
+      <c r="O10">
+        <v>100</v>
+      </c>
+      <c r="P10">
+        <v>100</v>
+      </c>
+      <c r="Q10">
+        <v>100</v>
+      </c>
+      <c r="R10">
+        <v>100</v>
+      </c>
+      <c r="S10">
+        <v>100</v>
+      </c>
+      <c r="T10">
+        <v>100</v>
+      </c>
+      <c r="U10">
+        <v>100</v>
+      </c>
+      <c r="V10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11">
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <v>1.5002</v>
+      </c>
+      <c r="E11">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F11">
+        <v>0.374</v>
+      </c>
+      <c r="G11">
+        <v>0.379</v>
+      </c>
+      <c r="H11">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="I11">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="J11">
+        <v>0.24399999999999999</v>
+      </c>
+      <c r="K11">
+        <v>0.192</v>
+      </c>
+      <c r="L11">
+        <v>0.155</v>
+      </c>
+      <c r="M11">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="N11">
+        <v>100</v>
+      </c>
+      <c r="O11">
+        <v>100</v>
+      </c>
+      <c r="P11">
+        <v>100</v>
+      </c>
+      <c r="Q11">
+        <v>100</v>
+      </c>
+      <c r="R11">
+        <v>100</v>
+      </c>
+      <c r="S11">
+        <v>100</v>
+      </c>
+      <c r="T11">
+        <v>100</v>
+      </c>
+      <c r="U11">
+        <v>100</v>
+      </c>
+      <c r="V11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="1">
+        <v>3.3250000000000002</v>
+      </c>
+      <c r="M12" s="1">
+        <v>3.0459999999999998</v>
+      </c>
+      <c r="N12">
+        <v>50</v>
+      </c>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+      <c r="U12">
+        <v>10</v>
+      </c>
+      <c r="V12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>0.05</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="K13" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="L13" s="1">
+        <v>2.5950000000000002</v>
+      </c>
+      <c r="M13" s="1">
+        <v>2.48</v>
+      </c>
+      <c r="N13" s="1">
+        <v>50</v>
+      </c>
+      <c r="O13" s="1">
+        <v>50</v>
+      </c>
+      <c r="P13" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>50</v>
+      </c>
+      <c r="R13" s="1">
+        <v>50</v>
+      </c>
+      <c r="S13" s="1">
+        <v>50</v>
+      </c>
+      <c r="T13" s="1">
+        <v>20</v>
+      </c>
+      <c r="U13" s="1">
+        <v>10</v>
+      </c>
+      <c r="V13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14">
+        <v>200</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.86899999999999999</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="K14" s="1">
+        <v>1.115</v>
+      </c>
+      <c r="L14" s="1">
+        <v>1.8129999999999999</v>
+      </c>
+      <c r="M14" s="1">
+        <v>1.536</v>
+      </c>
+      <c r="N14" s="1">
+        <v>50</v>
+      </c>
+      <c r="O14" s="1">
+        <v>50</v>
+      </c>
+      <c r="P14" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>50</v>
+      </c>
+      <c r="R14" s="1">
+        <v>50</v>
+      </c>
+      <c r="S14" s="1">
+        <v>50</v>
+      </c>
+      <c r="T14" s="1">
+        <v>20</v>
+      </c>
+      <c r="U14" s="1">
+        <v>10</v>
+      </c>
+      <c r="V14" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+      <c r="D15">
+        <v>0.2</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0.754</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.223</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.314</v>
+      </c>
+      <c r="L15" s="1">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.11</v>
+      </c>
+      <c r="N15" s="1">
+        <v>50</v>
+      </c>
+      <c r="O15" s="1">
+        <v>50</v>
+      </c>
+      <c r="P15" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>50</v>
+      </c>
+      <c r="R15" s="1">
+        <v>50</v>
+      </c>
+      <c r="S15" s="1">
+        <v>50</v>
+      </c>
+      <c r="T15" s="1">
+        <v>20</v>
+      </c>
+      <c r="U15" s="1">
+        <v>10</v>
+      </c>
+      <c r="V15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+      <c r="D16">
+        <v>0.3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.89200000000000002</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.66700000000000004</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.57799999999999996</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="J16" s="1">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="K16" s="1">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="L16" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="M16" s="1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N16" s="1">
+        <v>50</v>
+      </c>
+      <c r="O16" s="1">
+        <v>50</v>
+      </c>
+      <c r="P16" s="1">
+        <v>50</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>50</v>
+      </c>
+      <c r="R16" s="1">
+        <v>50</v>
+      </c>
+      <c r="S16" s="1">
+        <v>50</v>
+      </c>
+      <c r="T16" s="1">
+        <v>20</v>
+      </c>
+      <c r="U16" s="1">
+        <v>10</v>
+      </c>
+      <c r="V16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17">
+        <v>400</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1.655</v>
+      </c>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="1">
+        <v>1.6559999999999999</v>
+      </c>
+      <c r="M17" s="1">
+        <v>1.712</v>
+      </c>
+      <c r="N17" s="1">
+        <v>50.5</v>
+      </c>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="1">
+        <v>50</v>
+      </c>
+      <c r="V17" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18">
+        <v>400</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1.677</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0.81699999999999995</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.71099999999999997</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1.2549999999999999</v>
+      </c>
+      <c r="M18" s="1">
+        <v>1.2789999999999999</v>
+      </c>
+      <c r="N18" s="1">
+        <v>50.5</v>
+      </c>
+      <c r="O18" s="1">
+        <v>100</v>
+      </c>
+      <c r="P18" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>100</v>
+      </c>
+      <c r="R18" s="1">
+        <v>100</v>
+      </c>
+      <c r="S18" s="1">
+        <v>100</v>
+      </c>
+      <c r="T18" s="1">
+        <v>100</v>
+      </c>
+      <c r="U18" s="1">
+        <v>50</v>
+      </c>
+      <c r="V18" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19">
+        <v>400</v>
+      </c>
+      <c r="D19">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1.6319999999999999</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0.74099999999999999</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="L19" s="1">
+        <v>0.76900000000000002</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="N19" s="1">
+        <v>50.5</v>
+      </c>
+      <c r="O19" s="1">
+        <v>100</v>
+      </c>
+      <c r="P19" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>100</v>
+      </c>
+      <c r="R19" s="1">
+        <v>100</v>
+      </c>
+      <c r="S19" s="1">
+        <v>100</v>
+      </c>
+      <c r="T19" s="1">
+        <v>100</v>
+      </c>
+      <c r="U19" s="1">
+        <v>50</v>
+      </c>
+      <c r="V19" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20">
+        <v>400</v>
+      </c>
+      <c r="D20">
+        <v>0.3</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1.5149999999999999</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="M20" s="1">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="N20" s="1">
+        <v>50.5</v>
+      </c>
+      <c r="O20" s="1">
+        <v>100</v>
+      </c>
+      <c r="P20" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>100</v>
+      </c>
+      <c r="R20" s="1">
+        <v>100</v>
+      </c>
+      <c r="S20" s="1">
+        <v>100</v>
+      </c>
+      <c r="T20" s="1">
+        <v>100</v>
+      </c>
+      <c r="U20" s="1">
+        <v>50</v>
+      </c>
+      <c r="V20" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="C21">
+        <v>400</v>
+      </c>
+      <c r="D21">
+        <v>0.4</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1.69</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0.54900000000000004</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="J21" s="1">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="K21" s="1">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="L21" s="1">
+        <v>0.105</v>
+      </c>
+      <c r="M21" s="1">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>50.5</v>
+      </c>
+      <c r="O21" s="1">
+        <v>100</v>
+      </c>
+      <c r="P21" s="1">
+        <v>100</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>100</v>
+      </c>
+      <c r="R21" s="1">
+        <v>100</v>
+      </c>
+      <c r="S21" s="1">
+        <v>100</v>
+      </c>
+      <c r="T21" s="1">
+        <v>100</v>
+      </c>
+      <c r="U21" s="1">
+        <v>50</v>
+      </c>
+      <c r="V21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:22">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:22">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:22">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:22">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:22">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:22">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:22">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:22">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:22">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="3:8">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added group4's MB calib data
</commit_message>
<xml_diff>
--- a/data_raw/input.xlsx
+++ b/data_raw/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nobuakiohsumi/Lec_handson/wtrwks_rpt/data_raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E73E04A-86C8-FC47-B7E0-5D3113089072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B53C8F-3F66-DE42-8D51-A7EF1C6A2F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="7" xr2:uid="{11D640DA-DCFB-E544-8ADF-BF4092E26F00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" activeTab="6" xr2:uid="{11D640DA-DCFB-E544-8ADF-BF4092E26F00}"/>
   </bookViews>
   <sheets>
     <sheet name="colony" sheetId="3" r:id="rId1"/>
@@ -460,7 +460,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -483,9 +483,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -9653,10 +9650,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10B8D198-DF4E-5A4D-80C0-879C2B2FE6E1}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="200" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -9883,6 +9880,104 @@
       </c>
       <c r="D16">
         <v>3.35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0.115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>5</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1.0549999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1.9339999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1">
+        <v>3.331</v>
       </c>
     </row>
   </sheetData>
@@ -9895,7 +9990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F043729-32A1-B842-8BA1-3C91CFC99C7F}">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="124" workbookViewId="0"/>
+    <sheetView zoomScale="124" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <sheetData>
@@ -9989,7 +10084,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="8">
+      <c r="L2">
         <v>0.92800000000000005</v>
       </c>
       <c r="M2">
@@ -10004,7 +10099,7 @@
       <c r="R2" s="4"/>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
-      <c r="U2" s="8">
+      <c r="U2">
         <v>100</v>
       </c>
       <c r="V2">
@@ -10946,12 +11041,12 @@
       <c r="N17" s="1">
         <v>50.5</v>
       </c>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-      <c r="T17" s="9"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="8"/>
       <c r="U17" s="1">
         <v>50</v>
       </c>

</xml_diff>